<commit_message>
deleted duplicate fastq files in 3357 and 3275, and corrected fastq fille in 4144 01.13.20
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_3357.xlsx
+++ b/bioSample/bioSample_3357.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205D4B86-69A7-DA4C-A1F1-0B7FBAC4ED8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F465046D-53CA-DE4F-9639-4317C35F8F36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="17220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="54">
   <si>
     <t>harvestDate</t>
   </si>
@@ -564,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -615,13 +615,13 @@
         <v>52</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -644,13 +644,13 @@
         <v>52</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -667,19 +667,19 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>52</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -691,7 +691,7 @@
         <v>90</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -702,13 +702,13 @@
         <v>52</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -731,13 +731,13 @@
         <v>52</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -754,19 +754,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>52</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -778,7 +778,7 @@
         <v>90</v>
       </c>
       <c r="I7">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -789,16 +789,16 @@
         <v>52</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
         <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -807,7 +807,7 @@
         <v>90</v>
       </c>
       <c r="I8">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -818,16 +818,16 @@
         <v>52</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
         <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -836,7 +836,7 @@
         <v>90</v>
       </c>
       <c r="I9">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -847,16 +847,16 @@
         <v>52</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -865,28 +865,28 @@
         <v>90</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>52</v>
       </c>
       <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
-      </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
@@ -894,7 +894,7 @@
         <v>90</v>
       </c>
       <c r="I11">
-        <v>7</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -905,16 +905,16 @@
         <v>52</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -923,7 +923,7 @@
         <v>90</v>
       </c>
       <c r="I12">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -934,16 +934,16 @@
         <v>52</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
         <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -952,7 +952,7 @@
         <v>90</v>
       </c>
       <c r="I13">
-        <v>27</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -963,16 +963,16 @@
         <v>52</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
         <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -992,16 +992,16 @@
         <v>52</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
         <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -1021,16 +1021,16 @@
         <v>52</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -1050,16 +1050,16 @@
         <v>52</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
         <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
@@ -1079,16 +1079,16 @@
         <v>52</v>
       </c>
       <c r="C18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
         <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
@@ -1108,16 +1108,16 @@
         <v>52</v>
       </c>
       <c r="C19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" t="s">
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -1137,16 +1137,16 @@
         <v>52</v>
       </c>
       <c r="C20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
         <v>11</v>
@@ -1166,16 +1166,16 @@
         <v>52</v>
       </c>
       <c r="C21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" t="s">
         <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
@@ -1195,16 +1195,16 @@
         <v>52</v>
       </c>
       <c r="C22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
         <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
@@ -1224,16 +1224,16 @@
         <v>52</v>
       </c>
       <c r="C23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
         <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
@@ -1253,16 +1253,16 @@
         <v>52</v>
       </c>
       <c r="C24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
         <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G24" t="s">
         <v>11</v>
@@ -1271,7 +1271,7 @@
         <v>90</v>
       </c>
       <c r="I24">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1282,16 +1282,16 @@
         <v>52</v>
       </c>
       <c r="C25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" t="s">
         <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G25" t="s">
         <v>11</v>
@@ -1311,16 +1311,16 @@
         <v>52</v>
       </c>
       <c r="C26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
         <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G26" t="s">
         <v>11</v>
@@ -1340,16 +1340,16 @@
         <v>52</v>
       </c>
       <c r="C27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27" t="s">
         <v>53</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
@@ -1358,7 +1358,7 @@
         <v>90</v>
       </c>
       <c r="I27">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1369,16 +1369,16 @@
         <v>52</v>
       </c>
       <c r="C28">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
         <v>53</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="G28" t="s">
         <v>11</v>
@@ -1387,32 +1387,6 @@
         <v>90</v>
       </c>
       <c r="I28">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29">
-        <v>28</v>
-      </c>
-      <c r="E29" t="s">
-        <v>16</v>
-      </c>
-      <c r="F29" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29">
-        <v>90</v>
-      </c>
-      <c r="I29">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added strain names run 2641 to 4019
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_3357.xlsx
+++ b/bioSample/bioSample_3357.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/bioSample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9F328D-5E99-0342-82FB-9F35ADA792D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B162FD-158F-2C41-9BA1-F4D76A37F528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="17220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,16 +177,16 @@
     <t>CNAG_02700</t>
   </si>
   <si>
-    <t>KN99alpha</t>
-  </si>
-  <si>
-    <t>KN99A</t>
-  </si>
-  <si>
     <t>H.BROWN</t>
   </si>
   <si>
     <t>90minuteinduction</t>
+  </si>
+  <si>
+    <t>TDY450</t>
+  </si>
+  <si>
+    <t>TDY451</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -612,16 +612,16 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -641,13 +641,13 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
@@ -670,16 +670,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
         <v>53</v>
-      </c>
-      <c r="E4" t="s">
-        <v>50</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -699,16 +699,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -728,16 +728,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>7</v>
       </c>
       <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
         <v>53</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -757,13 +757,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -786,13 +786,13 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -815,13 +815,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
@@ -844,16 +844,16 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>11</v>
       </c>
       <c r="D10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
         <v>53</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -873,13 +873,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -902,13 +902,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
         <v>20</v>
@@ -931,13 +931,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <v>14</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
@@ -960,13 +960,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
         <v>24</v>
@@ -989,13 +989,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15">
         <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>26</v>
@@ -1018,13 +1018,13 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s">
         <v>28</v>
@@ -1047,13 +1047,13 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17">
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
         <v>30</v>
@@ -1076,13 +1076,13 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18">
         <v>19</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1105,13 +1105,13 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C19">
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
@@ -1134,13 +1134,13 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20">
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
         <v>36</v>
@@ -1163,13 +1163,13 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21">
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
         <v>38</v>
@@ -1192,13 +1192,13 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C22">
         <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
         <v>40</v>
@@ -1221,13 +1221,13 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23">
         <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
         <v>42</v>
@@ -1250,13 +1250,13 @@
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
         <v>44</v>
@@ -1279,13 +1279,13 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25">
         <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E25" t="s">
         <v>46</v>
@@ -1308,13 +1308,13 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26">
         <v>27</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
         <v>48</v>
@@ -1337,13 +1337,13 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C27">
         <v>28</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>

</xml_diff>